<commit_message>
Update README.md and other files
</commit_message>
<xml_diff>
--- a/Custodians_Results_1748952115.xlsx
+++ b/Custodians_Results_1748952115.xlsx
@@ -20607,8 +20607,10 @@
           <t>closing price: 26.78</t>
         </is>
       </c>
-      <c r="M220" s="50" t="n">
-        <v>4340000</v>
+      <c r="M220" s="50" t="inlineStr">
+        <is>
+          <t>Error: All extraction methods failed</t>
+        </is>
       </c>
       <c r="N220" s="5" t="n"/>
       <c r="P220" s="4" t="inlineStr">
@@ -20693,7 +20695,7 @@
       </c>
       <c r="M221" s="52" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>145</t>
         </is>
       </c>
       <c r="P221" s="1" t="inlineStr">
@@ -20784,7 +20786,7 @@
       </c>
       <c r="M222" s="44" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>100000</t>
         </is>
       </c>
       <c r="O222" s="20" t="n"/>
@@ -20871,7 +20873,7 @@
       </c>
       <c r="M223" s="52" t="inlineStr">
         <is>
-          <t>777</t>
+          <t>56839000 (AI)</t>
         </is>
       </c>
       <c r="P223" s="28" t="inlineStr">
@@ -21238,7 +21240,7 @@
       </c>
       <c r="M227" s="46" t="inlineStr">
         <is>
-          <t>37017000</t>
+          <t>37142000</t>
         </is>
       </c>
       <c r="N227" s="5" t="n"/>
@@ -21331,7 +21333,7 @@
       </c>
       <c r="M228" s="45" t="inlineStr">
         <is>
-          <t>37017000</t>
+          <t>37142000</t>
         </is>
       </c>
       <c r="N228" s="33" t="inlineStr">
@@ -21426,7 +21428,7 @@
       </c>
       <c r="M229" s="46" t="inlineStr">
         <is>
-          <t>61328000</t>
+          <t>61228000</t>
         </is>
       </c>
       <c r="N229" s="5" t="n"/>
@@ -21519,7 +21521,7 @@
       </c>
       <c r="M230" s="45" t="inlineStr">
         <is>
-          <t>61328000</t>
+          <t>61228000</t>
         </is>
       </c>
       <c r="N230" s="33" t="inlineStr">
@@ -21616,7 +21618,7 @@
       </c>
       <c r="M231" s="56" t="inlineStr">
         <is>
-          <t>61328000</t>
+          <t>61228000</t>
         </is>
       </c>
       <c r="N231" s="35" t="inlineStr">
@@ -22163,7 +22165,7 @@
       </c>
       <c r="M237" s="47" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>935000</t>
         </is>
       </c>
       <c r="P237" s="28" t="inlineStr">
@@ -22251,7 +22253,7 @@
       </c>
       <c r="M238" s="47" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>125000</t>
         </is>
       </c>
       <c r="P238" s="28" t="inlineStr">
@@ -22337,7 +22339,7 @@
       </c>
       <c r="M239" s="47" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>47600 (AI)</t>
         </is>
       </c>
       <c r="P239" s="28" t="inlineStr">
@@ -22423,7 +22425,7 @@
       </c>
       <c r="M240" s="47" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>100000</t>
         </is>
       </c>
       <c r="P240" s="28" t="inlineStr">
@@ -22509,7 +22511,7 @@
       </c>
       <c r="M241" s="47" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>185000</t>
         </is>
       </c>
       <c r="P241" s="28" t="inlineStr">
@@ -22686,7 +22688,7 @@
       </c>
       <c r="M243" s="47" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>2090000</t>
         </is>
       </c>
       <c r="P243" s="1" t="inlineStr">
@@ -23214,7 +23216,7 @@
       </c>
       <c r="M249" s="44" t="inlineStr">
         <is>
-          <t>56839 (AI)</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="P249" s="4" t="inlineStr">
@@ -23560,7 +23562,7 @@
       </c>
       <c r="M253" s="44" t="inlineStr">
         <is>
-          <t>56839 (AI)</t>
+          <t>56839000 (AI)</t>
         </is>
       </c>
       <c r="P253" s="4" t="inlineStr">
@@ -24492,7 +24494,7 @@
       </c>
       <c r="M264" s="44" t="inlineStr">
         <is>
-          <t>56839 (AI)</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="P264" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Add existing project files and updates
</commit_message>
<xml_diff>
--- a/Custodians_Results_1748952115.xlsx
+++ b/Custodians_Results_1748952115.xlsx
@@ -1007,7 +1007,7 @@
       </c>
       <c r="M1" s="43" t="inlineStr">
         <is>
-          <t>Outstanding shares (Last updated: 2025-06-03 07:38:16)</t>
+          <t>Outstanding shares (Last updated: 2025-06-03 17:06:51)</t>
         </is>
       </c>
       <c r="N1" s="22" t="inlineStr">
@@ -25972,7 +25972,7 @@
       </c>
       <c r="M281" s="91" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>56839 (AI)</t>
         </is>
       </c>
       <c r="P281" s="4" t="inlineStr">
@@ -27263,7 +27263,7 @@
       </c>
       <c r="M296" s="46" t="inlineStr">
         <is>
-          <t>8285000</t>
+          <t>56839000 (AI)</t>
         </is>
       </c>
       <c r="P296" s="1" t="inlineStr">
@@ -27552,8 +27552,10 @@
           <t>closing price prev trading day: 3.9525</t>
         </is>
       </c>
-      <c r="M299" s="46" t="n">
-        <v>30</v>
+      <c r="M299" s="46" t="inlineStr">
+        <is>
+          <t>Error: All extraction methods failed</t>
+        </is>
       </c>
       <c r="P299" s="1" t="inlineStr">
         <is>
@@ -27649,7 +27651,7 @@
       </c>
       <c r="M300" s="44" t="inlineStr">
         <is>
-          <t>56839 (AI)</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="O300" s="42" t="n"/>
@@ -27827,7 +27829,7 @@
       </c>
       <c r="M302" s="44" t="inlineStr">
         <is>
-          <t>56839 (AI)</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="O302" s="42" t="n"/>
@@ -27916,7 +27918,7 @@
       </c>
       <c r="M303" s="44" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>56839 (AI)</t>
         </is>
       </c>
       <c r="O303" s="42" t="n"/>
@@ -28091,7 +28093,7 @@
       </c>
       <c r="M305" s="46" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>27500 (AI)</t>
         </is>
       </c>
       <c r="P305" s="30" t="inlineStr">
@@ -28791,7 +28793,7 @@
       </c>
       <c r="M313" s="44" t="inlineStr">
         <is>
-          <t>56839000 (AI)</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="P313" s="16" t="inlineStr">
@@ -30262,7 +30264,7 @@
       </c>
       <c r="M330" s="100" t="inlineStr">
         <is>
-          <t>49,725,000</t>
+          <t>49,625,000</t>
         </is>
       </c>
       <c r="P330" s="28" t="inlineStr">
@@ -30352,7 +30354,7 @@
       </c>
       <c r="M331" s="100" t="inlineStr">
         <is>
-          <t>74,650,000</t>
+          <t>74,775,000</t>
         </is>
       </c>
       <c r="P331" s="28" t="inlineStr">
@@ -30442,7 +30444,7 @@
       </c>
       <c r="M332" s="100" t="inlineStr">
         <is>
-          <t>24,150,000</t>
+          <t>24,125,000</t>
         </is>
       </c>
       <c r="P332" s="28" t="inlineStr">
@@ -30973,7 +30975,7 @@
       </c>
       <c r="M338" s="100" t="inlineStr">
         <is>
-          <t>20,325,000</t>
+          <t>20,350,000</t>
         </is>
       </c>
       <c r="P338" s="28" t="inlineStr">
@@ -31999,7 +32001,7 @@
       </c>
       <c r="M350" s="47" t="inlineStr">
         <is>
-          <t>5243332</t>
+          <t>Error: All extraction methods failed</t>
         </is>
       </c>
       <c r="P350" s="23" t="inlineStr">
@@ -33421,7 +33423,7 @@
       </c>
       <c r="M377" s="105" t="inlineStr">
         <is>
-          <t>Error: All extraction methods failed</t>
+          <t>45415000</t>
         </is>
       </c>
       <c r="N377" s="103" t="inlineStr">

</xml_diff>